<commit_message>
edited codebook, added csv
</commit_message>
<xml_diff>
--- a/codebook_kimelodie.xlsx
+++ b/codebook_kimelodie.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Desktop\uni\Master\Projektarbeit\Supplement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5709288B-A1C3-4BB1-A7A5-716465A5DCB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7296AB2-4D8A-4DB9-A94A-BE26290AA6A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="17115" windowHeight="10755" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="59">
   <si>
     <t>Variable</t>
   </si>
@@ -139,12 +139,6 @@
     <t>HK* / KH*</t>
   </si>
   <si>
-    <t>definitly human</t>
-  </si>
-  <si>
-    <t>definitly machine</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -170,13 +164,46 @@
   </si>
   <si>
     <t>More than 10 years.</t>
+  </si>
+  <si>
+    <t>Codebook: The Performance of Creative AI Systems</t>
+  </si>
+  <si>
+    <t>ID and Consent</t>
+  </si>
+  <si>
+    <t>Rating Items; Note: Every Melody was rated with the same four items (starting with "F"), the appendix (e.g. "01") refers to the specific rating variable</t>
+  </si>
+  <si>
+    <t>Decision items; Note: AI compositions</t>
+  </si>
+  <si>
+    <t>definitly human [1]</t>
+  </si>
+  <si>
+    <t>[4]</t>
+  </si>
+  <si>
+    <t>[5]</t>
+  </si>
+  <si>
+    <t>[6]</t>
+  </si>
+  <si>
+    <t>[7]</t>
+  </si>
+  <si>
+    <t>definitly machine [8]</t>
+  </si>
+  <si>
+    <t>Sociodemographic variables</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -197,13 +224,37 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -227,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -247,6 +298,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -561,11 +624,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="4" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -579,117 +642,69 @@
     <col min="7" max="1024" width="11.46484375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.4">
+      <c r="A1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="14"/>
+    </row>
+    <row r="3" spans="1:6" s="12" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+    <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B6" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>13</v>
@@ -697,19 +712,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2">
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>13</v>
@@ -717,90 +732,64 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="6"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" s="12" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="11"/>
+    </row>
+    <row r="11" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="C8" s="2">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="2">
-        <v>4</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="2">
-        <v>5</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="2">
-        <v>-9</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
@@ -815,12 +804,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C13" s="2">
         <v>2</v>
@@ -835,12 +824,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C14" s="2">
         <v>3</v>
@@ -855,12 +844,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C15" s="2">
         <v>4</v>
@@ -875,12 +864,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C16" s="2">
         <v>5</v>
@@ -895,12 +884,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C17" s="2">
         <v>-9</v>
@@ -915,12 +904,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C18" s="5">
         <v>1</v>
@@ -935,12 +924,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C19" s="2">
         <v>2</v>
@@ -955,12 +944,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C20" s="2">
         <v>3</v>
@@ -975,12 +964,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C21" s="2">
         <v>4</v>
@@ -995,12 +984,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C22" s="2">
         <v>5</v>
@@ -1015,12 +1004,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C23" s="2">
         <v>-9</v>
@@ -1037,10 +1026,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C24" s="5">
         <v>1</v>
@@ -1057,10 +1046,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C25" s="2">
         <v>2</v>
@@ -1077,10 +1066,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C26" s="2">
         <v>3</v>
@@ -1097,10 +1086,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C27" s="2">
         <v>4</v>
@@ -1117,10 +1106,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C28" s="2">
         <v>5</v>
@@ -1137,10 +1126,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C29" s="2">
         <v>-9</v>
@@ -1155,18 +1144,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" s="5">
         <v>1</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>14</v>
@@ -1175,18 +1164,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>14</v>
@@ -1195,18 +1184,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C32" s="2">
-        <v>-9</v>
+        <v>3</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>14</v>
@@ -1216,40 +1205,40 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="5">
-        <v>1</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" s="4" t="s">
+      <c r="A33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="2">
+        <v>4</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C34" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>13</v>
@@ -1257,137 +1246,437 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="2">
+        <v>-9</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="6"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" s="12" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="11"/>
+    </row>
+    <row r="38" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A38" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="5">
+        <v>1</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="18">
+        <v>2</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="18">
+        <v>3</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="18">
+        <v>4</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="18">
+        <v>5</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="18">
+        <v>6</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="18">
+        <v>7</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="2">
+        <v>8</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="2">
+        <v>-9</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="12" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="11"/>
+    </row>
+    <row r="50" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A50" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B51" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C51" s="5">
+        <v>1</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" s="2">
+        <v>2</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="2">
+      <c r="E52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C53" s="2">
         <v>3</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C54" s="2">
+        <v>-9</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="38.25" x14ac:dyDescent="0.35">
+      <c r="A56" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="C56" s="5">
+        <v>1</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E56" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" s="2">
+      <c r="F56" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="38.25" x14ac:dyDescent="0.35">
+      <c r="A57" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C57" s="2">
+        <v>2</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="38.25" x14ac:dyDescent="0.35">
+      <c r="A58" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C58" s="2">
+        <v>3</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="38.25" x14ac:dyDescent="0.35">
+      <c r="A59" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C59" s="2">
         <v>-9</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="38.25" x14ac:dyDescent="0.35">
-      <c r="A38" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="5">
-        <v>1</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="38.25" x14ac:dyDescent="0.35">
-      <c r="A39" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="2">
-        <v>2</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="38.25" x14ac:dyDescent="0.35">
-      <c r="A40" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" s="2">
-        <v>3</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="38.25" x14ac:dyDescent="0.35">
-      <c r="A41" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" s="2">
-        <v>-9</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F41" s="1" t="s">
+      <c r="F59" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>